<commit_message>
ponto neutro e cm_alfa - aeronave altamente instável
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\consu\Documents\manuel\projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC9492F1-8B9F-45FC-814D-40F821811D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBA0979-6603-4E68-8CE5-09496E6E87C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>1+rt</t>
   </si>
@@ -68,13 +68,70 @@
   </si>
   <si>
     <t>xcm</t>
+  </si>
+  <si>
+    <t>asa frente</t>
+  </si>
+  <si>
+    <t>asa trás</t>
+  </si>
+  <si>
+    <t>pos asa/ fuselagem</t>
+  </si>
+  <si>
+    <t>para ft com x=2.5</t>
+  </si>
+  <si>
+    <t>pos asa fuselagem = 0.7</t>
+  </si>
+  <si>
+    <t>temos estabilidade, mas provavelmente estamos só a sonhar alto demais</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>aw</t>
+  </si>
+  <si>
+    <t>[/rad]</t>
+  </si>
+  <si>
+    <t>h_nw</t>
+  </si>
+  <si>
+    <t>lht</t>
+  </si>
+  <si>
+    <t>e_alfa</t>
+  </si>
+  <si>
+    <t>hn</t>
+  </si>
+  <si>
+    <t>xpn</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>Cl_alfa</t>
+  </si>
+  <si>
+    <t>[/grau]</t>
+  </si>
+  <si>
+    <t>cm_alfa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,13 +139,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,8 +174,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,15 +493,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
-  <dimension ref="F4:K19"/>
+  <dimension ref="E4:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:15" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -435,7 +509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>2</v>
       </c>
@@ -449,8 +523,14 @@
         <f>G5*H5</f>
         <v>348</v>
       </c>
-    </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>2</v>
       </c>
@@ -465,7 +545,7 @@
         <v>477.59999999999997</v>
       </c>
     </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>2</v>
       </c>
@@ -479,23 +559,28 @@
         <f t="shared" si="0"/>
         <v>607.20000000000005</v>
       </c>
-    </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <f>G7-G6</f>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="8" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8">
-        <v>5.2450000000000001</v>
+        <f>L7+G7</f>
+        <v>4.6050000000000004</v>
       </c>
       <c r="H8">
         <v>160</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>839.2</v>
-      </c>
-    </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.25">
+        <v>736.80000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>2</v>
       </c>
@@ -510,7 +595,7 @@
         <v>968.8</v>
       </c>
     </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>0</v>
       </c>
@@ -526,7 +611,7 @@
         <v>1235.7</v>
       </c>
     </row>
-    <row r="11" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>3</v>
       </c>
@@ -537,15 +622,16 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I17" si="1">G11*H11</f>
+        <f t="shared" ref="I11:I19" si="1">G11*H11</f>
         <v>597</v>
       </c>
     </row>
-    <row r="12" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>4</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
+        <f>1.5 + O5 +1</f>
         <v>2.7</v>
       </c>
       <c r="H12">
@@ -556,22 +642,23 @@
         <v>378</v>
       </c>
     </row>
-    <row r="13" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="G13">
-        <v>6.1</v>
+        <f>G12 + (1-O5 + 3)</f>
+        <v>6.5</v>
       </c>
       <c r="H13">
         <v>140</v>
       </c>
       <c r="I13">
         <f t="shared" si="1"/>
-        <v>854</v>
-      </c>
-    </row>
-    <row r="14" spans="6:9" x14ac:dyDescent="0.25">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>6</v>
       </c>
@@ -586,7 +673,7 @@
         <v>3752.4500000000003</v>
       </c>
     </row>
-    <row r="15" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>8</v>
       </c>
@@ -601,7 +688,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="16" spans="6:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>7</v>
       </c>
@@ -615,42 +702,184 @@
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.25">
+      <c r="O16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17">
+        <f>G12</f>
+        <v>2.7</v>
+      </c>
+      <c r="H17">
+        <v>200</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ref="I17" si="2">G17*H17</f>
+        <v>540</v>
+      </c>
+      <c r="O17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18">
+        <f>G13</f>
+        <v>6.5</v>
+      </c>
+      <c r="H18">
+        <v>200</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
         <v>9</v>
       </c>
-      <c r="G17">
-        <v>4.4074999999999998</v>
-      </c>
-      <c r="H17">
+      <c r="G19" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H19">
         <v>2200</v>
       </c>
-      <c r="I17">
+      <c r="I19">
         <f t="shared" si="1"/>
-        <v>9696.5</v>
-      </c>
-    </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="H18">
-        <f>SUM(H5:H17)</f>
-        <v>4680</v>
-      </c>
-      <c r="I18">
-        <f>SUM(I5:I17)</f>
-        <v>20329.45</v>
-      </c>
-      <c r="K18" t="s">
+        <v>9680</v>
+      </c>
+    </row>
+    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f>SUM(H5:H19)</f>
+        <v>5080</v>
+      </c>
+      <c r="I20">
+        <f>SUM(I5:I19)</f>
+        <v>22106.55</v>
+      </c>
+      <c r="K20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.25">
-      <c r="K19">
-        <f>I18/H18</f>
-        <v>4.3438995726495726</v>
+    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>I20/H20</f>
+        <v>4.3516830708661418</v>
+      </c>
+    </row>
+    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23">
+        <f>(F26 + (F27/F23 + F26)*(1-F28))/(1+(1-F28))</f>
+        <v>0.9624999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <f>1.5+O5</f>
+        <v>1.7</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="3">
+        <f>F24+J23*F23</f>
+        <v>3.6249999999999996</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25">
+        <f>0.106</f>
+        <v>0.106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>0.25</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="3">
+        <f>(J24-K21)/F23</f>
+        <v>-0.36334153543307113</v>
+      </c>
+    </row>
+    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27">
+        <f>(1-O5)+3</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28">
+        <v>0.4</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J28" s="3">
+        <f>F25+F25*(1-F28)</f>
+        <v>0.16959999999999997</v>
+      </c>
+      <c r="K28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="3">
+        <f>-J26*J28</f>
+        <v>6.1622724409448854E-2</v>
+      </c>
+      <c r="K29" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sem comentário da Rafa
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBA0979-6603-4E68-8CE5-09496E6E87C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCDDFE2-7D28-4A13-B3C1-144DFD81D877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>1+rt</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>pos asa fuselagem = 0.7</t>
-  </si>
-  <si>
-    <t>temos estabilidade, mas provavelmente estamos só a sonhar alto demais</t>
   </si>
   <si>
     <t>c</t>
@@ -197,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,13 +492,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
   <dimension ref="E4:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:15" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -509,7 +506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F5">
         <v>2</v>
       </c>
@@ -530,7 +527,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F6">
         <v>2</v>
       </c>
@@ -545,7 +542,7 @@
         <v>477.59999999999997</v>
       </c>
     </row>
-    <row r="7" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F7">
         <v>2</v>
       </c>
@@ -564,7 +561,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="8" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F8">
         <v>2</v>
       </c>
@@ -580,7 +577,7 @@
         <v>736.80000000000007</v>
       </c>
     </row>
-    <row r="9" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F9">
         <v>2</v>
       </c>
@@ -595,7 +592,7 @@
         <v>968.8</v>
       </c>
     </row>
-    <row r="10" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
         <v>0</v>
       </c>
@@ -611,7 +608,7 @@
         <v>1235.7</v>
       </c>
     </row>
-    <row r="11" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>3</v>
       </c>
@@ -626,7 +623,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="12" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
         <v>4</v>
       </c>
@@ -642,7 +639,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="13" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
         <v>5</v>
       </c>
@@ -658,7 +655,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
         <v>6</v>
       </c>
@@ -673,7 +670,7 @@
         <v>3752.4500000000003</v>
       </c>
     </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
         <v>8</v>
       </c>
@@ -688,7 +685,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
         <v>7</v>
       </c>
@@ -706,7 +703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
         <v>11</v>
       </c>
@@ -725,7 +722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
         <v>12</v>
       </c>
@@ -740,11 +737,8 @@
         <f t="shared" si="1"/>
         <v>1300</v>
       </c>
-      <c r="O18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
         <v>9</v>
       </c>
@@ -759,7 +753,7 @@
         <v>9680</v>
       </c>
     </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
       <c r="H20">
         <f>SUM(H5:H19)</f>
         <v>5080</v>
@@ -772,37 +766,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
       <c r="K21">
         <f>I20/H20</f>
         <v>4.3516830708661418</v>
       </c>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J23">
         <f>(F26 + (F27/F23 + F26)*(1-F28))/(1+(1-F28))</f>
         <v>0.9624999999999998</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F24">
         <f>1.5+O5</f>
         <v>1.7</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J24" s="3">
         <f>F24+J23*F23</f>
@@ -812,70 +806,70 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25">
         <f>0.106</f>
         <v>0.106</v>
       </c>
       <c r="G25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="E26" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="E26" t="s">
-        <v>21</v>
       </c>
       <c r="F26">
         <v>0.25</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J26" s="3">
         <f>(J24-K21)/F23</f>
         <v>-0.36334153543307113</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27">
         <f>(1-O5)+3</f>
         <v>3.8</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28">
         <v>0.4</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J28" s="3">
         <f>F25+F25*(1-F28)</f>
         <v>0.16959999999999997</v>
       </c>
       <c r="K28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="I29" s="3" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="3" t="s">
-        <v>29</v>
       </c>
       <c r="J29" s="3">
         <f>-J26*J28</f>
         <v>6.1622724409448854E-2</v>
       </c>
       <c r="K29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novo cm e ponto neutro
temos estabilidade forçada, mas temos
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCDDFE2-7D28-4A13-B3C1-144DFD81D877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2056678B-9DE6-437B-9956-CDA82BA6473E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>1+rt</t>
   </si>
@@ -94,9 +94,6 @@
     <t>aw</t>
   </si>
   <si>
-    <t>[/rad]</t>
-  </si>
-  <si>
     <t>h_nw</t>
   </si>
   <si>
@@ -122,6 +119,42 @@
   </si>
   <si>
     <t>cm_alfa</t>
+  </si>
+  <si>
+    <t>45cm entre "parede" da roda e banco</t>
+  </si>
+  <si>
+    <t>temos 80 cm para a parte das rodas</t>
+  </si>
+  <si>
+    <t>fuselagem</t>
+  </si>
+  <si>
+    <t>centro fuselagem</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>cone 1</t>
+  </si>
+  <si>
+    <t>centro</t>
+  </si>
+  <si>
+    <t>cone 2</t>
+  </si>
+  <si>
+    <t>xcfus</t>
+  </si>
+  <si>
+    <t>posi. 1ª asa</t>
+  </si>
+  <si>
+    <t>considerado pelo prof como distancia entre bordo da primeira asa e ponto neutro da segunda</t>
+  </si>
+  <si>
+    <t>valor muito exagerado???</t>
   </si>
 </sst>
 </file>
@@ -194,7 +227,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -490,15 +523,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
-  <dimension ref="E4:O29"/>
+  <dimension ref="D4:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="6:20" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -506,19 +542,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5">
-        <v>2.1749999999999998</v>
+        <f>2.175-0.5</f>
+        <v>1.6749999999999998</v>
       </c>
       <c r="H5">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I5">
         <f>G5*H5</f>
-        <v>348</v>
+        <v>334.99999999999994</v>
       </c>
       <c r="M5" t="s">
         <v>13</v>
@@ -526,78 +563,138 @@
       <c r="O5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="6" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>2.9849999999999999</v>
+        <f>G5+0.81</f>
+        <v>2.4849999999999999</v>
       </c>
       <c r="H6">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I9" si="0">G6*H6</f>
-        <v>477.59999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="6:15" x14ac:dyDescent="0.3">
+        <v>497</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>2</v>
       </c>
       <c r="G7">
-        <v>3.7949999999999999</v>
+        <f t="shared" ref="G7:G8" si="1">G6+0.81</f>
+        <v>3.2949999999999999</v>
       </c>
       <c r="H7">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>607.20000000000005</v>
+        <v>659</v>
       </c>
       <c r="L7">
         <f>G7-G6</f>
         <v>0.81</v>
       </c>
-    </row>
-    <row r="8" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="Q7" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7">
+        <v>0.67</v>
+      </c>
+      <c r="S7">
+        <f>1*2.25*0.5</f>
+        <v>1.125</v>
+      </c>
+      <c r="T7">
+        <f>R7*S7</f>
+        <v>0.75375000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>2</v>
       </c>
       <c r="G8">
-        <f>L7+G7</f>
-        <v>4.6050000000000004</v>
+        <f t="shared" si="1"/>
+        <v>4.1050000000000004</v>
       </c>
       <c r="H8">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>736.80000000000007</v>
-      </c>
-    </row>
-    <row r="9" spans="6:15" x14ac:dyDescent="0.3">
+        <v>821.00000000000011</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8">
+        <f>1+6.5/2</f>
+        <v>4.25</v>
+      </c>
+      <c r="S8">
+        <f>2.25*6.5</f>
+        <v>14.625</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ref="T8:T9" si="2">R8*S8</f>
+        <v>62.15625</v>
+      </c>
+    </row>
+    <row r="9" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <v>6.0549999999999997</v>
+        <f>6.025</f>
+        <v>6.0250000000000004</v>
       </c>
       <c r="H9">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>968.8</v>
-      </c>
-    </row>
-    <row r="10" spans="6:15" x14ac:dyDescent="0.3">
+        <v>1205</v>
+      </c>
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>35</v>
+      </c>
+      <c r="R9">
+        <f>6.5+1.5/3</f>
+        <v>7</v>
+      </c>
+      <c r="S9">
+        <f>(2.25*1.5)/2</f>
+        <v>1.6875</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>11.8125</v>
+      </c>
+    </row>
+    <row r="10" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>0</v>
       </c>
       <c r="G10">
-        <v>6.8650000000000002</v>
+        <f>7.025</f>
+        <v>7.0250000000000004</v>
       </c>
       <c r="H10">
         <f>80+100</f>
@@ -605,124 +702,138 @@
       </c>
       <c r="I10">
         <f>G10*H10</f>
-        <v>1235.7</v>
-      </c>
-    </row>
-    <row r="11" spans="6:15" x14ac:dyDescent="0.3">
+        <v>1264.5</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10">
+        <f>SUM(S7:S9)</f>
+        <v>17.4375</v>
+      </c>
+    </row>
+    <row r="11" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11">
-        <v>2.9849999999999999</v>
+        <f>2.1</f>
+        <v>2.1</v>
       </c>
       <c r="H11">
         <v>200</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I19" si="1">G11*H11</f>
-        <v>597</v>
-      </c>
-    </row>
-    <row r="12" spans="6:15" x14ac:dyDescent="0.3">
+        <f t="shared" ref="I11:I20" si="3">G11*H11</f>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="12" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="1">
-        <f>1.5 + O5 +1</f>
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="H12">
         <v>140</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="13" spans="6:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>420</v>
+      </c>
+      <c r="S12" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12">
+        <f>SUM(T7:T9)/S10</f>
+        <v>4.2851612903225806</v>
+      </c>
+    </row>
+    <row r="13" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="G13">
-        <f>G12 + (1-O5 + 3)</f>
         <v>6.5</v>
       </c>
       <c r="H13">
         <v>140</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>910</v>
       </c>
     </row>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>6</v>
       </c>
       <c r="G14">
-        <v>8.1575000000000006</v>
+        <v>8</v>
       </c>
       <c r="H14">
         <v>460</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
-        <v>3752.4500000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="15" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H15">
         <v>510</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>510</v>
-      </c>
-    </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="16" spans="6:20" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>7</v>
       </c>
       <c r="G16">
-        <v>1.3</v>
+        <f>1-0.28/2</f>
+        <v>0.86</v>
       </c>
       <c r="H16">
         <v>50</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
-        <v>65</v>
+        <f t="shared" si="3"/>
+        <v>43</v>
       </c>
       <c r="O16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>11</v>
       </c>
       <c r="G17">
         <f>G12</f>
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="H17">
         <v>200</v>
       </c>
       <c r="I17">
-        <f t="shared" ref="I17" si="2">G17*H17</f>
-        <v>540</v>
+        <f t="shared" ref="I17" si="4">G17*H17</f>
+        <v>600</v>
       </c>
       <c r="O17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F18" t="s">
         <v>12</v>
       </c>
@@ -734,142 +845,172 @@
         <v>200</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1300</v>
       </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19">
+        <f>T12</f>
+        <v>4.2851612903225806</v>
+      </c>
+      <c r="H19">
+        <v>800</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>3428.1290322580644</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H19">
+      <c r="G20" s="2">
+        <f>2.25</f>
+        <v>2.25</v>
+      </c>
+      <c r="H20">
         <v>2200</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>9680</v>
-      </c>
-    </row>
-    <row r="20" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="H20">
-        <f>SUM(H5:H19)</f>
-        <v>5080</v>
-      </c>
       <c r="I20">
-        <f>SUM(I5:I19)</f>
-        <v>22106.55</v>
+        <f t="shared" si="3"/>
+        <v>4950</v>
       </c>
       <c r="K20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f>SUM(H5:H20)</f>
+        <v>6080</v>
+      </c>
+      <c r="I21">
+        <f>SUM(I5:I20)</f>
+        <v>20787.629032258064</v>
+      </c>
+      <c r="K21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="K21">
-        <f>I20/H20</f>
-        <v>4.3516830708661418</v>
-      </c>
-    </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E23" t="s">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f>I21/H21</f>
+        <v>3.4190179329371815</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="F23">
+      <c r="F24">
         <v>2</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I24" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24">
+        <f>(F27 + (F28/F24)*(1-F29))/(1+(1-F29))</f>
+        <v>0.90624999999999989</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25">
+        <f>G17-1</f>
+        <v>2</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J23">
-        <f>(F26 + (F27/F23 + F26)*(1-F28))/(1+(1-F28))</f>
-        <v>0.9624999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24">
-        <f>1.5+O5</f>
-        <v>1.7</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J24" s="3">
-        <f>F24+J23*F23</f>
-        <v>3.6249999999999996</v>
-      </c>
-      <c r="K24" t="s">
+      <c r="J25" s="3">
+        <f>F25+J24*F24</f>
+        <v>3.8125</v>
+      </c>
+      <c r="K25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E25" t="s">
+      <c r="L25">
+        <f>J25-K22</f>
+        <v>0.39348206706281852</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
         <v>18</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <f>0.106</f>
         <v>0.106</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E26" t="s">
+      <c r="F27">
+        <v>0.25</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="3">
+        <f>(J25-K22)/(2*F24)</f>
+        <v>9.837051676570463E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
         <v>20</v>
       </c>
-      <c r="F26">
-        <v>0.25</v>
-      </c>
-      <c r="I26" s="3" t="s">
+      <c r="F28">
+        <f>G18-G17+F24*F27</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29">
+        <v>0.4</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="3">
-        <f>(J24-K21)/F23</f>
-        <v>-0.36334153543307113</v>
-      </c>
-    </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27">
-        <f>(1-O5)+3</f>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E28" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28">
-        <v>0.4</v>
-      </c>
-      <c r="I28" s="3" t="s">
+      <c r="J29" s="3">
+        <f>F26+F26*(1-F29)</f>
+        <v>0.16959999999999997</v>
+      </c>
+      <c r="K29" t="s">
         <v>26</v>
       </c>
-      <c r="J28" s="3">
-        <f>F25+F25*(1-F28)</f>
-        <v>0.16959999999999997</v>
-      </c>
-      <c r="K28" t="s">
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="I29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J29" s="3">
-        <f>-J26*J28</f>
-        <v>6.1622724409448854E-2</v>
-      </c>
-      <c r="K29" t="s">
-        <v>27</v>
+      <c r="J30" s="3">
+        <f>-J27*J29</f>
+        <v>-1.6683639643463501E-2</v>
+      </c>
+      <c r="K30" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novo cm e ponto neutro pt. 2
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC91C685-6773-4492-91AD-E06335F58041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59DA25C-2E18-4C12-9B53-665D217B9A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>bat+av</t>
   </si>
   <si>
-    <t>ft</t>
-  </si>
-  <si>
     <t>xcm</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Fuel Tanks</t>
+  </si>
+  <si>
+    <t>dist entre asas &gt; 2</t>
   </si>
 </sst>
 </file>
@@ -221,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -229,15 +229,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,7 +308,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -554,16 +606,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
   <dimension ref="D4:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -571,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>2</v>
       </c>
@@ -587,16 +639,16 @@
         <v>334.99999999999994</v>
       </c>
       <c r="M5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O5">
         <v>0.2</v>
       </c>
       <c r="R5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>2</v>
       </c>
@@ -615,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>2</v>
       </c>
@@ -638,7 +690,7 @@
         <v>0.81</v>
       </c>
       <c r="Q7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R7">
         <v>0.67</v>
@@ -652,7 +704,7 @@
         <v>0.75375000000000003</v>
       </c>
     </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>2</v>
       </c>
@@ -668,7 +720,7 @@
         <v>821.00000000000011</v>
       </c>
       <c r="Q8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R8">
         <f>1+6.5/2</f>
@@ -683,26 +735,26 @@
         <v>62.15625</v>
       </c>
     </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>2</v>
       </c>
       <c r="G9">
-        <f>6.025</f>
-        <v>6.0250000000000004</v>
+        <f>G8+0.81</f>
+        <v>4.9150000000000009</v>
       </c>
       <c r="H9">
         <v>200</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>1205</v>
+        <v>983.00000000000023</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R9">
         <f>6.5+1.5/3</f>
@@ -717,9 +769,9 @@
         <v>11.8125</v>
       </c>
     </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>0</v>
@@ -737,75 +789,78 @@
         <v>1264.5</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S10">
         <f>SUM(S7:S9)</f>
         <v>17.4375</v>
       </c>
     </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11">
-        <f>2.1</f>
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="H11">
         <v>200</v>
       </c>
       <c r="I11">
         <f t="shared" ref="I11:I20" si="3">G11*H11</f>
-        <v>420</v>
-      </c>
-    </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="1">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H12">
         <v>140</v>
       </c>
       <c r="I12">
         <f t="shared" si="3"/>
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="S12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T12">
         <f>SUM(T7:T9)/S10</f>
         <v>4.2851612903225806</v>
       </c>
     </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
       </c>
       <c r="G13">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="H13">
         <v>140</v>
       </c>
       <c r="I13">
         <f t="shared" si="3"/>
-        <v>910</v>
-      </c>
-    </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
+        <v>1050</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
@@ -820,10 +875,15 @@
         <f t="shared" si="3"/>
         <v>3680</v>
       </c>
-    </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
+      <c r="K14" s="6">
+        <f>G13-G12-F24</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -839,9 +899,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
         <v>7</v>
@@ -858,56 +918,56 @@
         <v>43</v>
       </c>
       <c r="O16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G17">
         <f>G12</f>
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="H17">
         <v>200</v>
       </c>
       <c r="I17">
         <f t="shared" ref="I17" si="4">G17*H17</f>
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="O17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18">
         <f>G13</f>
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="H18">
         <v>200</v>
       </c>
       <c r="I18">
         <f t="shared" si="3"/>
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19">
         <f>T12</f>
@@ -921,158 +981,149 @@
         <v>3428.1290322580644</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="2">
-        <f>2.25</f>
-        <v>2.25</v>
-      </c>
-      <c r="H20">
-        <v>2200</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="3"/>
-        <v>4950</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="G20" s="2"/>
       <c r="K20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H21">
         <f>SUM(H5:H20)</f>
-        <v>6080</v>
+        <v>3880</v>
       </c>
       <c r="I21">
         <f>SUM(I5:I20)</f>
-        <v>20787.629032258064</v>
+        <v>15949.629032258064</v>
       </c>
       <c r="K21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="K22">
         <f>I21/H21</f>
-        <v>3.4190179329371815</v>
-      </c>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+        <v>4.1107291320252743</v>
+      </c>
+      <c r="O22" s="2"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J24">
         <f>(F27 + (F28/F24)*(1-F29))/(1+(1-F29))</f>
-        <v>0.90624999999999989</v>
-      </c>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+        <v>1.075</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25">
         <f>G17-1</f>
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J25" s="3">
         <f>F25+J24*F24</f>
-        <v>3.8125</v>
+        <v>4.25</v>
       </c>
       <c r="K25" t="s">
         <v>2</v>
       </c>
       <c r="L25">
         <f>J25-K22</f>
-        <v>0.39348206706281852</v>
-      </c>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+        <v>0.13927086797472565</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F26">
         <f>0.106</f>
         <v>0.106</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27">
         <v>0.25</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J27" s="3">
         <f>(J25-K22)/(2*F24)</f>
-        <v>9.837051676570463E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+        <v>3.4817716993681413E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28">
         <f>G18-G17+F24*F27</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F29">
         <v>0.4</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J29" s="3">
         <f>F26+F26*(1-F29)</f>
         <v>0.16959999999999997</v>
       </c>
       <c r="K29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="I30" s="3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="I30" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="J30" s="3">
         <f>-J27*J29</f>
-        <v>-1.6683639643463501E-2</v>
+        <v>-5.9050848021283669E-3</v>
       </c>
       <c r="K30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="K14:L14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Algumas alterações para fazer o Snip
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59DA25C-2E18-4C12-9B53-665D217B9A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61191CBE-A9AA-4730-A110-06EA73465E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -308,7 +308,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -606,16 +606,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
   <dimension ref="D4:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -623,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F5">
         <v>2</v>
       </c>
@@ -648,7 +648,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F6">
         <v>2</v>
       </c>
@@ -670,7 +670,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F7">
         <v>2</v>
       </c>
@@ -704,7 +704,7 @@
         <v>0.75375000000000003</v>
       </c>
     </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F8">
         <v>2</v>
       </c>
@@ -735,7 +735,7 @@
         <v>62.15625</v>
       </c>
     </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F9">
         <v>2</v>
       </c>
@@ -769,7 +769,7 @@
         <v>11.8125</v>
       </c>
     </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>39</v>
       </c>
@@ -796,7 +796,7 @@
         <v>17.4375</v>
       </c>
     </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>3</v>
       </c>
@@ -807,11 +807,11 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I20" si="3">G11*H11</f>
+        <f t="shared" ref="I11:I19" si="3">G11*H11</f>
         <v>380</v>
       </c>
     </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>40</v>
       </c>
@@ -836,7 +836,7 @@
         <v>4.2851612903225806</v>
       </c>
     </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -858,7 +858,7 @@
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>42</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>43</v>
       </c>
@@ -899,7 +899,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>44</v>
       </c>
@@ -921,7 +921,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>45</v>
       </c>
@@ -943,7 +943,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>46</v>
       </c>
@@ -962,7 +962,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>47</v>
       </c>
@@ -981,16 +981,16 @@
         <v>3428.1290322580644</v>
       </c>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>48</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
       <c r="H21">
         <f>SUM(H5:H20)</f>
         <v>3880</v>
@@ -1003,14 +1003,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K22">
         <f>I21/H21</f>
         <v>4.1107291320252743</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>1.075</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>36</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>0.13927086797472565</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>17</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>18</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>3.4817716993681413E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
       <c r="I30" s="3" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
add estabilizador vertical para cm
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61191CBE-A9AA-4730-A110-06EA73465E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E8EF30-1430-44C7-8319-F6BC68630C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="0" yWindow="840" windowWidth="12450" windowHeight="9870" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
   <si>
     <t>1+rt</t>
   </si>
@@ -180,10 +180,16 @@
     <t>Fuselagem</t>
   </si>
   <si>
-    <t>Fuel Tanks</t>
-  </si>
-  <si>
     <t>dist entre asas &gt; 2</t>
+  </si>
+  <si>
+    <t>vertical tail</t>
+  </si>
+  <si>
+    <t>vt</t>
+  </si>
+  <si>
+    <t>[/rad]</t>
   </si>
 </sst>
 </file>
@@ -308,7 +314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -604,18 +610,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
-  <dimension ref="D4:T30"/>
+  <dimension ref="D4:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -623,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>2</v>
       </c>
@@ -648,7 +654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>2</v>
       </c>
@@ -670,7 +676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>2</v>
       </c>
@@ -704,7 +710,7 @@
         <v>0.75375000000000003</v>
       </c>
     </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>2</v>
       </c>
@@ -735,7 +741,7 @@
         <v>62.15625</v>
       </c>
     </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>2</v>
       </c>
@@ -769,7 +775,7 @@
         <v>11.8125</v>
       </c>
     </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>39</v>
       </c>
@@ -796,7 +802,7 @@
         <v>17.4375</v>
       </c>
     </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>3</v>
       </c>
@@ -807,11 +813,11 @@
         <v>200</v>
       </c>
       <c r="I11">
-        <f t="shared" ref="I11:I19" si="3">G11*H11</f>
+        <f t="shared" ref="I11:I20" si="3">G11*H11</f>
         <v>380</v>
       </c>
     </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>40</v>
       </c>
@@ -836,7 +842,7 @@
         <v>4.2851612903225806</v>
       </c>
     </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -854,11 +860,11 @@
         <v>1050</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>42</v>
       </c>
@@ -881,7 +887,7 @@
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>43</v>
       </c>
@@ -899,7 +905,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>44</v>
       </c>
@@ -921,7 +927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>45</v>
       </c>
@@ -943,7 +949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>46</v>
       </c>
@@ -962,7 +968,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>47</v>
       </c>
@@ -974,43 +980,56 @@
         <v>4.2851612903225806</v>
       </c>
       <c r="H19">
-        <v>800</v>
+        <v>405.25</v>
       </c>
       <c r="I19">
         <f t="shared" si="3"/>
-        <v>3428.1290322580644</v>
-      </c>
-    </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
+        <v>1736.5616129032258</v>
+      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="H20">
+        <v>50</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>425</v>
+      </c>
       <c r="L20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
       <c r="H21">
         <f>SUM(H5:H20)</f>
-        <v>3880</v>
+        <v>3535.25</v>
       </c>
       <c r="I21">
         <f>SUM(I5:I20)</f>
-        <v>15949.629032258064</v>
+        <v>14683.061612903226</v>
       </c>
       <c r="K21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
       <c r="K22">
         <f>I21/H21</f>
-        <v>4.1107291320252743</v>
+        <v>4.1533304894712471</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1044,7 @@
         <v>1.075</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
         <v>36</v>
       </c>
@@ -1048,10 +1067,10 @@
       </c>
       <c r="L25">
         <f>J25-K22</f>
-        <v>0.13927086797472565</v>
-      </c>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
+        <v>9.6669510528752944E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>17</v>
       </c>
@@ -1063,7 +1082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>18</v>
       </c>
@@ -1075,10 +1094,10 @@
       </c>
       <c r="J27" s="3">
         <f>(J25-K22)/(2*F24)</f>
-        <v>3.4817716993681413E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
+        <v>2.4167377632188236E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1090,7 +1109,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -1108,16 +1127,25 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="I30" s="3" t="s">
         <v>26</v>
       </c>
       <c r="J30" s="3">
         <f>-J27*J29</f>
-        <v>-5.9050848021283669E-3</v>
+        <v>-4.0987872464191243E-3</v>
       </c>
       <c r="K30" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f>J30*180/PI()</f>
+        <v>-0.23484321034186395</v>
+      </c>
+      <c r="K31" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
C_L_alpha em rad e plano de evacuação
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w\Documents\GitHub\ProjetoIntegrador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E8EF30-1430-44C7-8319-F6BC68630C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F9D946-5EE9-45E2-A9EA-8F50DD0DB649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="12450" windowHeight="9870" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
   <si>
     <t>1+rt</t>
   </si>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -613,15 +613,15 @@
   <dimension ref="D4:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:20" x14ac:dyDescent="0.3">
       <c r="G4" t="s">
         <v>1</v>
       </c>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F5">
         <v>2</v>
       </c>
@@ -654,7 +654,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F6">
         <v>2</v>
       </c>
@@ -676,7 +676,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F7">
         <v>2</v>
       </c>
@@ -710,7 +710,7 @@
         <v>0.75375000000000003</v>
       </c>
     </row>
-    <row r="8" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F8">
         <v>2</v>
       </c>
@@ -741,7 +741,7 @@
         <v>62.15625</v>
       </c>
     </row>
-    <row r="9" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F9">
         <v>2</v>
       </c>
@@ -775,7 +775,7 @@
         <v>11.8125</v>
       </c>
     </row>
-    <row r="10" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
         <v>39</v>
       </c>
@@ -802,7 +802,7 @@
         <v>17.4375</v>
       </c>
     </row>
-    <row r="11" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:20" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
         <v>3</v>
       </c>
@@ -817,7 +817,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="12" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>40</v>
       </c>
@@ -842,7 +842,7 @@
         <v>4.2851612903225806</v>
       </c>
     </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -864,7 +864,7 @@
       </c>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>42</v>
       </c>
@@ -887,7 +887,7 @@
       </c>
       <c r="L14" s="7"/>
     </row>
-    <row r="15" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>43</v>
       </c>
@@ -905,7 +905,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:20" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>44</v>
       </c>
@@ -927,7 +927,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>45</v>
       </c>
@@ -949,7 +949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>46</v>
       </c>
@@ -968,7 +968,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>47</v>
       </c>
@@ -988,7 +988,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>49</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:15" x14ac:dyDescent="0.3">
       <c r="H21">
         <f>SUM(H5:H20)</f>
         <v>3535.25</v>
@@ -1022,14 +1022,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:15" x14ac:dyDescent="0.3">
       <c r="K22">
         <f>I21/H21</f>
         <v>4.1533304894712471</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E24" t="s">
         <v>15</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>1.075</v>
       </c>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D25" t="s">
         <v>36</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>9.6669510528752944E-2</v>
       </c>
     </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
         <v>17</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E27" t="s">
         <v>18</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>2.4167377632188236E-2</v>
       </c>
     </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:15" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>37</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -1126,8 +1126,15 @@
       <c r="K29" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <f>J29*180/PI()</f>
+        <v>9.717364205418761</v>
+      </c>
+      <c r="M29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.3">
       <c r="I30" s="3" t="s">
         <v>26</v>
       </c>
@@ -1139,7 +1146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:15" x14ac:dyDescent="0.3">
       <c r="J31">
         <f>J30*180/PI()</f>
         <v>-0.23484321034186395</v>

</xml_diff>

<commit_message>
Adimensionalização com duas cordas
Estamos com uma margem estática de 10%, afinal.
</commit_message>
<xml_diff>
--- a/calculocm.xlsx
+++ b/calculocm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Duarte\IST\2021-2022\2º Semestre\Projeto Integrador\ProjetoIntegrador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F9D946-5EE9-45E2-A9EA-8F50DD0DB649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F2C395-D988-497D-87E0-1F2515122F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{40763E0D-57AA-406A-8EBA-27EADA9E1614}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>1+rt</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>[/rad]</t>
+  </si>
+  <si>
+    <t>2c</t>
   </si>
 </sst>
 </file>
@@ -612,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E745EB7C-68B5-409A-A2FF-55C5E529EB64}">
   <dimension ref="D4:T31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1036,12 +1039,15 @@
       <c r="F24">
         <v>2</v>
       </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
       <c r="I24" t="s">
         <v>21</v>
       </c>
       <c r="J24">
-        <f>(F27 + (F28/F24)*(1-F29))/(1+(1-F29))</f>
-        <v>1.075</v>
+        <f>(F27 + (F28/F31)*(1-F29))/(1+(1-F29))</f>
+        <v>0.61562499999999998</v>
       </c>
     </row>
     <row r="25" spans="4:15" x14ac:dyDescent="0.3">
@@ -1055,19 +1061,22 @@
         <f>G17-1</f>
         <v>2.1</v>
       </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
       <c r="I25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="3">
-        <f>F25+J24*F24</f>
-        <v>4.25</v>
+        <f>F25+J24*F31</f>
+        <v>4.5625</v>
       </c>
       <c r="K25" t="s">
         <v>2</v>
       </c>
       <c r="L25">
         <f>J25-K22</f>
-        <v>9.6669510528752944E-2</v>
+        <v>0.40916951052875294</v>
       </c>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.3">
@@ -1094,7 +1103,7 @@
       </c>
       <c r="J27" s="3">
         <f>(J25-K22)/(2*F24)</f>
-        <v>2.4167377632188236E-2</v>
+        <v>0.10229237763218824</v>
       </c>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.3">
@@ -1108,6 +1117,9 @@
         <f>G18-G17+F24*F27</f>
         <v>4.9000000000000004</v>
       </c>
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
@@ -1140,16 +1152,26 @@
       </c>
       <c r="J30" s="3">
         <f>-J27*J29</f>
-        <v>-4.0987872464191243E-3</v>
+        <v>-1.7348787246419122E-2</v>
       </c>
       <c r="K30" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31">
+        <f>2*F24</f>
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2</v>
+      </c>
       <c r="J31">
         <f>J30*180/PI()</f>
-        <v>-0.23484321034186395</v>
+        <v>-0.99401228889020454</v>
       </c>
       <c r="K31" t="s">
         <v>51</v>

</xml_diff>